<commit_message>
add loger and logic for search in alternative region
</commit_message>
<xml_diff>
--- a/data/Книга1.xlsx
+++ b/data/Книга1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="473" yWindow="2543" windowWidth="21105" windowHeight="10860" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="выгрузка_PU" sheetId="1" state="visible" r:id="rId1"/>
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -37,18 +37,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00CCFFCC"/>
         <bgColor rgb="00CCFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFCCCC"/>
-        <bgColor rgb="00FFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CCDDFF"/>
-        <bgColor rgb="00CCDDFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -64,11 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -466,10 +452,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -484,132 +470,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>02/056719</t>
+          <t>07/048574</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>02/056712</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>нет</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>02/056718</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>01/186495</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>нет</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>01/186499</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>01/186490</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>05/050201</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>05/050198</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>04/124232</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>нет</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>07/128353</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>нет</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Ч-054040</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>07/048192</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>07/128351</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>нет</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>01/234218</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>нет</t>
-        </is>
-      </c>
-    </row>
-    <row r="16"/>
+    <row r="3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
add models, tests for services and services/
</commit_message>
<xml_diff>
--- a/data/Книга1.xlsx
+++ b/data/Книга1.xlsx
@@ -1,43 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code_on_python\AnalyticsAIAgent\AnalyticsAIAgent\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63BBE14-2512-4BAA-878A-3A611C1326A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="473" yWindow="2543" windowWidth="21105" windowHeight="10860" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="135" yWindow="2205" windowWidth="21105" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="выгрузка_PU" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="выгрузка_PU" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+  <si>
+    <t>Номера</t>
+  </si>
+  <si>
+    <t>07/048574</t>
+  </si>
+  <si>
+    <t>02/048574</t>
+  </si>
+  <si>
+    <t>04/048574</t>
+  </si>
+  <si>
+    <t>06/048574</t>
+  </si>
+  <si>
+    <t>Ч-048574</t>
+  </si>
+  <si>
+    <t>Б-048574</t>
+  </si>
+  <si>
+    <t>И-048574</t>
+  </si>
+  <si>
+    <t>К-048574</t>
+  </si>
+  <si>
+    <t>Н-048574</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CCFFCC"/>
-        <bgColor rgb="00CCFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,82 +86,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -447,36 +421,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Номера</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>07/048574</t>
-        </is>
-      </c>
-    </row>
-    <row r="3"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>